<commit_message>
removed hard coded path to excel file
</commit_message>
<xml_diff>
--- a/ILabApplication/Default.xlsx
+++ b/ILabApplication/Default.xlsx
@@ -219,10 +219,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -532,11 +532,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="11.93359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.2265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.10546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.97265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.93359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.2265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.10546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.97265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -554,13 +554,13 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>6</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>4</v>
       </c>
-      <c s="2">
+      <c s="1">
         <v>834725363</v>
       </c>
       <c s="3" t="s">
@@ -582,7 +582,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>
@@ -601,7 +601,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
added steps to function library
</commit_message>
<xml_diff>
--- a/ILabApplication/Default.xlsx
+++ b/ILabApplication/Default.xlsx
@@ -219,10 +219,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -532,11 +532,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="11.93359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.2265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.10546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.97265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.93359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.2265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.10546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.97265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -554,13 +554,13 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>6</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>4</v>
       </c>
-      <c s="1">
+      <c s="2">
         <v>834725363</v>
       </c>
       <c s="3" t="s">
@@ -582,7 +582,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>
@@ -601,7 +601,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>